<commit_message>
Master User 50 Persen
</commit_message>
<xml_diff>
--- a/Documents/Catatan.xlsx
+++ b/Documents/Catatan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="747" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="747" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Analisa" sheetId="13" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Inventory-Clinic" sheetId="10" r:id="rId13"/>
     <sheet name="Inventory-Warehouse" sheetId="11" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1328,6 +1328,12 @@
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1352,14 +1358,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1370,6 +1370,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1379,18 +1382,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="?蟓%U?&amp;H?_x0008__x001e__x000a_?_x000f__x0001__x0001_ 3" xfId="2"/>
@@ -1402,6 +1402,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2104,7 +2107,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2112,6 +2115,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2247,7 +2264,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2255,6 +2272,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2435,7 +2466,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2443,6 +2474,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2576,7 +2621,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2584,6 +2629,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2667,7 +2726,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2675,6 +2734,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2824,7 +2897,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2832,6 +2905,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2865,7 +2952,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2873,6 +2960,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3022,7 +3123,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3030,6 +3131,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3063,7 +3178,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3071,6 +3186,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3345,7 +3474,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3353,6 +3482,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -4260,7 +4403,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4295,7 +4438,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5139,43 +5282,43 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20" t="s">
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
       <c r="F8" s="3" t="s">
         <v>149</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="H8" s="20"/>
+      <c r="H8" s="26"/>
       <c r="I8" s="5" t="s">
         <v>170</v>
       </c>
@@ -5263,16 +5406,16 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="20" t="s">
+      <c r="C15" s="28"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
@@ -5351,43 +5494,43 @@
       <c r="B22" t="s">
         <v>169</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20" t="s">
+      <c r="H22" s="26"/>
+      <c r="I22" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="J22" s="21" t="s">
+      <c r="J22" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="K22" s="22"/>
-      <c r="L22" s="23"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="25"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="20"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="19"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="3" t="s">
         <v>149</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="I23" s="20"/>
+      <c r="I23" s="26"/>
       <c r="J23" s="3" t="s">
         <v>170</v>
       </c>
@@ -5488,16 +5631,16 @@
       <c r="B29" t="s">
         <v>179</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="24" t="s">
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="G29" s="25"/>
-      <c r="H29" s="26"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="29"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C30" s="3" t="s">
@@ -5585,43 +5728,43 @@
       <c r="B36" t="s">
         <v>169</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="E36" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="F36" s="18" t="s">
+      <c r="F36" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="G36" s="20" t="s">
+      <c r="G36" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20" t="s">
+      <c r="H36" s="26"/>
+      <c r="I36" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="J36" s="21" t="s">
+      <c r="J36" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="K36" s="22"/>
-      <c r="L36" s="23"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="25"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C37" s="20"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="19"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="3" t="s">
         <v>149</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="I37" s="20"/>
+      <c r="I37" s="26"/>
       <c r="J37" s="3" t="s">
         <v>170</v>
       </c>
@@ -5734,16 +5877,16 @@
       <c r="B43" t="s">
         <v>179</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="D43" s="25"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="24" t="s">
+      <c r="D43" s="28"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="G43" s="25"/>
-      <c r="H43" s="26"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="29"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C44" s="3" t="s">
@@ -5786,15 +5929,15 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C46" s="12" t="str">
+      <c r="C46" s="16" t="str">
         <f>C39</f>
         <v>Paramex</v>
       </c>
-      <c r="D46" s="12">
+      <c r="D46" s="16">
         <f>I39</f>
         <v>120</v>
       </c>
-      <c r="E46" s="12">
+      <c r="E46" s="16">
         <f>SUM(K39:K41)</f>
         <v>120</v>
       </c>
@@ -5812,9 +5955,9 @@
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
       <c r="F47" s="3" t="str">
         <f t="shared" ref="F47:F48" si="1">J40</f>
         <v>Panadol</v>
@@ -5829,9 +5972,9 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
       <c r="F48" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Paramet</v>
@@ -5873,43 +6016,43 @@
       <c r="B52" t="s">
         <v>169</v>
       </c>
-      <c r="C52" s="20" t="s">
+      <c r="C52" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D52" s="18" t="s">
+      <c r="D52" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="E52" s="20" t="s">
+      <c r="E52" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="F52" s="18" t="s">
+      <c r="F52" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="G52" s="20" t="s">
+      <c r="G52" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20" t="s">
+      <c r="H52" s="26"/>
+      <c r="I52" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="J52" s="21" t="s">
+      <c r="J52" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="K52" s="22"/>
-      <c r="L52" s="23"/>
+      <c r="K52" s="24"/>
+      <c r="L52" s="25"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C53" s="20"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="19"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="31"/>
       <c r="G53" s="3" t="s">
         <v>149</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="I53" s="20"/>
+      <c r="I53" s="26"/>
       <c r="J53" s="3" t="s">
         <v>170</v>
       </c>
@@ -6022,16 +6165,16 @@
       <c r="B59" t="s">
         <v>179</v>
       </c>
-      <c r="C59" s="24" t="s">
+      <c r="C59" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="D59" s="25"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="24" t="s">
+      <c r="D59" s="28"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="G59" s="25"/>
-      <c r="H59" s="26"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="29"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C60" s="3" t="s">
@@ -6074,15 +6217,15 @@
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C62" s="12" t="str">
+      <c r="C62" s="16" t="str">
         <f>C55</f>
         <v>Paramex</v>
       </c>
-      <c r="D62" s="12">
+      <c r="D62" s="16">
         <f>I55</f>
         <v>120</v>
       </c>
-      <c r="E62" s="12">
+      <c r="E62" s="16">
         <f>SUM(K55:K57)</f>
         <v>120</v>
       </c>
@@ -6100,9 +6243,9 @@
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
       <c r="F63" s="3" t="str">
         <f t="shared" ref="F63:F64" si="6">J56</f>
         <v>Panadol</v>
@@ -6117,9 +6260,9 @@
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
       <c r="F64" s="3" t="str">
         <f t="shared" si="6"/>
         <v>Paramet</v>
@@ -6153,43 +6296,43 @@
       <c r="B68" t="s">
         <v>169</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D68" s="18" t="s">
+      <c r="D68" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="E68" s="20" t="s">
+      <c r="E68" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="F68" s="18" t="s">
+      <c r="F68" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="G68" s="20" t="s">
+      <c r="G68" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="H68" s="20"/>
-      <c r="I68" s="20" t="s">
+      <c r="H68" s="26"/>
+      <c r="I68" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="J68" s="21" t="s">
+      <c r="J68" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="K68" s="22"/>
-      <c r="L68" s="23"/>
+      <c r="K68" s="24"/>
+      <c r="L68" s="25"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C69" s="20"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="19"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="31"/>
       <c r="G69" s="3" t="s">
         <v>149</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="I69" s="20"/>
+      <c r="I69" s="26"/>
       <c r="J69" s="3" t="s">
         <v>170</v>
       </c>
@@ -6302,16 +6445,16 @@
       <c r="B75" t="s">
         <v>179</v>
       </c>
-      <c r="C75" s="24" t="s">
+      <c r="C75" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="D75" s="25"/>
-      <c r="E75" s="26"/>
-      <c r="F75" s="24" t="s">
+      <c r="D75" s="28"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="G75" s="25"/>
-      <c r="H75" s="26"/>
+      <c r="G75" s="28"/>
+      <c r="H75" s="29"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C76" s="3" t="s">
@@ -6354,15 +6497,15 @@
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C78" s="12" t="str">
+      <c r="C78" s="16" t="str">
         <f>C71</f>
         <v>Paramex</v>
       </c>
-      <c r="D78" s="12">
+      <c r="D78" s="16">
         <f>I71</f>
         <v>120</v>
       </c>
-      <c r="E78" s="12">
+      <c r="E78" s="16">
         <f>SUM(K71:K73)</f>
         <v>170</v>
       </c>
@@ -6380,9 +6523,9 @@
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="13"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
       <c r="F79" s="3" t="str">
         <f t="shared" ref="F79:F80" si="9">J72</f>
         <v>Panadol</v>
@@ -6397,9 +6540,9 @@
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
       <c r="F80" s="3" t="str">
         <f t="shared" si="9"/>
         <v>Paramet</v>
@@ -6423,6 +6566,45 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="E78:E80"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="I68:I69"/>
+    <mergeCell ref="J68:L68"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="E62:E64"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="J52:L52"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G22:H22"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="J36:L36"/>
     <mergeCell ref="E15:G15"/>
@@ -6438,45 +6620,6 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="J52:L52"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="I68:I69"/>
-    <mergeCell ref="J68:L68"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="D62:D64"/>
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="E78:E80"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="G68:H68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6484,8 +6627,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11265" r:id="rId3" name="cmdsub">
+        <control shapeId="11275" r:id="rId3" name="CommandButton9">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>76200</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>12</xdr:col>
+                <xdr:colOff>247650</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="11275" r:id="rId3" name="CommandButton9"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="11274" r:id="rId5" name="CommandButton8">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>76</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>78</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="11274" r:id="rId5" name="CommandButton8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="11273" r:id="rId7" name="CommandButton7">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>12</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>69</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>219075</xdr:colOff>
+                <xdr:row>71</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="11273" r:id="rId7" name="CommandButton7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="11272" r:id="rId9" name="CommandButton6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>60</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>62</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="11272" r:id="rId9" name="CommandButton6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="11271" r:id="rId11" name="CommandButton5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>12</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>53</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>219075</xdr:colOff>
+                <xdr:row>55</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="11271" r:id="rId11" name="CommandButton5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="11270" r:id="rId13" name="CommandButton4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>44</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>46</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="11270" r:id="rId13" name="CommandButton4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="11269" r:id="rId15" name="CommandButton3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>266700</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="11269" r:id="rId15" name="CommandButton3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="11268" r:id="rId17" name="CommandButton1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>219075</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="11268" r:id="rId17" name="CommandButton1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="11267" r:id="rId19" name="CommandButton2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>12</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>219075</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="11267" r:id="rId19" name="CommandButton2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="11265" r:id="rId21" name="cmdsub">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>12</xdr:col>
@@ -6504,232 +6872,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11265" r:id="rId3" name="cmdsub"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="11267" r:id="rId5" name="CommandButton2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>12</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>219075</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="11267" r:id="rId5" name="CommandButton2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="11268" r:id="rId7" name="CommandButton1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>219075</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="11268" r:id="rId7" name="CommandButton1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="11269" r:id="rId9" name="CommandButton3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>266700</xdr:colOff>
-                <xdr:row>32</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="11269" r:id="rId9" name="CommandButton3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="11270" r:id="rId11" name="CommandButton4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>44</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>46</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="11270" r:id="rId11" name="CommandButton4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="11271" r:id="rId13" name="CommandButton5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>12</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>53</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>219075</xdr:colOff>
-                <xdr:row>55</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="11271" r:id="rId13" name="CommandButton5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="11272" r:id="rId15" name="CommandButton6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>60</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>62</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="11272" r:id="rId15" name="CommandButton6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="11273" r:id="rId17" name="CommandButton7">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>12</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>69</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>219075</xdr:colOff>
-                <xdr:row>71</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="11273" r:id="rId17" name="CommandButton7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="11274" r:id="rId19" name="CommandButton8">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>76</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>78</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="11274" r:id="rId19" name="CommandButton8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="11275" r:id="rId21" name="CommandButton9">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>11</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>12</xdr:col>
-                <xdr:colOff>247650</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="11275" r:id="rId21" name="CommandButton9"/>
+        <control shapeId="11265" r:id="rId21" name="cmdsub"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -6843,28 +6986,28 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="10" t="s">
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="20" t="s">
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20" t="s">
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="O14" s="20"/>
+      <c r="O14" s="26"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -7036,28 +7179,28 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="10" t="s">
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="20" t="s">
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20" t="s">
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="O29" s="20"/>
+      <c r="O29" s="26"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
@@ -7295,24 +7438,24 @@
       <c r="C45" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D45" s="20">
+      <c r="D45" s="26">
         <v>1</v>
       </c>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20">
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26">
         <v>2</v>
       </c>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
       <c r="J45" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="K45" s="20" t="s">
+      <c r="K45" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="L45" s="20"/>
-      <c r="M45" s="20"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="26"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
@@ -7404,17 +7547,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="J14:M14"/>
     <mergeCell ref="N14:O14"/>
     <mergeCell ref="F14:I14"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="F29:I29"/>
     <mergeCell ref="J29:M29"/>
     <mergeCell ref="N29:O29"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="J14:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7441,7 +7584,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
@@ -7504,62 +7647,62 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="11" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="12" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="12" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="12" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="12" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="12" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="12" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="12" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="12" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="12" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="12" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="12" t="s">
         <v>309</v>
       </c>
     </row>
@@ -7567,7 +7710,7 @@
       <c r="A21">
         <v>8</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="12" t="s">
         <v>310</v>
       </c>
     </row>
@@ -7575,7 +7718,7 @@
       <c r="A22">
         <v>9</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="12" t="s">
         <v>311</v>
       </c>
     </row>
@@ -7583,7 +7726,7 @@
       <c r="A23">
         <v>10</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="12" t="s">
         <v>312</v>
       </c>
     </row>
@@ -7591,7 +7734,7 @@
       <c r="A24">
         <v>11</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="12" t="s">
         <v>313</v>
       </c>
     </row>
@@ -7599,7 +7742,7 @@
       <c r="A25">
         <v>12</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="12" t="s">
         <v>314</v>
       </c>
     </row>
@@ -7607,7 +7750,7 @@
       <c r="A26">
         <v>13</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="12" t="s">
         <v>317</v>
       </c>
     </row>
@@ -7615,7 +7758,7 @@
       <c r="A27">
         <v>14</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="12" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7623,7 +7766,7 @@
       <c r="A28">
         <v>15</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="12" t="s">
         <v>316</v>
       </c>
     </row>
@@ -7631,7 +7774,7 @@
       <c r="A29">
         <v>16</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="12" t="s">
         <v>318</v>
       </c>
     </row>
@@ -7639,7 +7782,7 @@
       <c r="A30">
         <v>17</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="12" t="s">
         <v>319</v>
       </c>
     </row>
@@ -7647,7 +7790,7 @@
       <c r="A31">
         <v>18</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="12" t="s">
         <v>320</v>
       </c>
     </row>
@@ -7655,7 +7798,7 @@
       <c r="A32">
         <v>19</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="12" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7663,7 +7806,7 @@
       <c r="A33">
         <v>20</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="12" t="s">
         <v>322</v>
       </c>
     </row>
@@ -7671,7 +7814,7 @@
       <c r="A34">
         <v>21</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="12" t="s">
         <v>323</v>
       </c>
     </row>
@@ -7679,7 +7822,7 @@
       <c r="A35">
         <v>22</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="12" t="s">
         <v>324</v>
       </c>
     </row>
@@ -7687,27 +7830,27 @@
       <c r="A36">
         <v>23</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="10" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="10" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="10" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="10" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="10" t="s">
         <v>329</v>
       </c>
     </row>
@@ -7715,27 +7858,27 @@
       <c r="A41">
         <v>24</v>
       </c>
-      <c r="B41" s="29" t="s">
+      <c r="B41" s="10" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="10" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="10" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="10" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="10" t="s">
         <v>352</v>
       </c>
     </row>
@@ -7743,22 +7886,22 @@
       <c r="A46">
         <v>25</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="10" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="10" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="10" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="29" t="s">
+      <c r="B49" s="10" t="s">
         <v>336</v>
       </c>
     </row>
@@ -7766,62 +7909,62 @@
       <c r="A50">
         <v>26</v>
       </c>
-      <c r="B50" s="29" t="s">
+      <c r="B50" s="10" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="10" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="32" t="s">
+      <c r="B52" s="13" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="32" t="s">
+      <c r="B53" s="13" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="32" t="s">
+      <c r="B54" s="13" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="32" t="s">
+      <c r="B55" s="13" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="13" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="32" t="s">
+      <c r="B57" s="13" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="13" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="32" t="s">
+      <c r="B59" s="13" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="32" t="s">
+      <c r="B60" s="13" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="32" t="s">
+      <c r="B61" s="13" t="s">
         <v>348</v>
       </c>
     </row>
@@ -7829,7 +7972,7 @@
       <c r="A62">
         <v>27</v>
       </c>
-      <c r="B62" s="32" t="s">
+      <c r="B62" s="13" t="s">
         <v>349</v>
       </c>
     </row>
@@ -7837,7 +7980,7 @@
       <c r="A63">
         <v>28</v>
       </c>
-      <c r="B63" s="32" t="s">
+      <c r="B63" s="13" t="s">
         <v>350</v>
       </c>
     </row>
@@ -7845,7 +7988,7 @@
       <c r="A64">
         <v>29</v>
       </c>
-      <c r="B64" s="32" t="s">
+      <c r="B64" s="13" t="s">
         <v>353</v>
       </c>
     </row>
@@ -8658,10 +8801,10 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="C53" s="11"/>
+      <c r="C53" s="15"/>
       <c r="D53" s="1" t="s">
         <v>111</v>
       </c>
@@ -8679,13 +8822,13 @@
       <c r="C54" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="E54" s="12">
+      <c r="E54" s="16">
         <v>13</v>
       </c>
-      <c r="F54" s="15" t="s">
+      <c r="F54" s="19" t="s">
         <v>114</v>
       </c>
     </row>
@@ -8696,9 +8839,9 @@
       <c r="C55" s="1">
         <v>6</v>
       </c>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="16"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="20"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
@@ -8707,9 +8850,9 @@
       <c r="C56" s="1">
         <v>3</v>
       </c>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="16"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="20"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
@@ -8718,9 +8861,9 @@
       <c r="C57" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="17"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>